<commit_message>
created add separate competitors by using form
</commit_message>
<xml_diff>
--- a/public/uploads/participants.xlsx
+++ b/public/uploads/participants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6. Mes projets\14.2. Symfony_competition-results\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83313CA-6ACE-42C3-97B2-250FECCE8FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16241CB-6E11-43AD-BD2B-CC974E4FFDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{A2BB81C9-9CA3-43A5-A119-25B82A2C596C}"/>
+    <workbookView xWindow="4188" yWindow="4188" windowWidth="23040" windowHeight="12600" xr2:uid="{A2BB81C9-9CA3-43A5-A119-25B82A2C596C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Mulhouse</t>
   </si>
@@ -136,6 +136,33 @@
   </si>
   <si>
     <t>jim@gmail.com</t>
+  </si>
+  <si>
+    <t>Doa</t>
+  </si>
+  <si>
+    <t>Dob</t>
+  </si>
+  <si>
+    <t>Doc</t>
+  </si>
+  <si>
+    <t>Dod</t>
+  </si>
+  <si>
+    <t>Dof</t>
+  </si>
+  <si>
+    <t>Dog</t>
+  </si>
+  <si>
+    <t>Doh</t>
+  </si>
+  <si>
+    <t>Doi</t>
+  </si>
+  <si>
+    <t>Doj</t>
   </si>
 </sst>
 </file>
@@ -492,7 +519,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,7 +548,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>25</v>
@@ -535,7 +562,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>26</v>
@@ -549,7 +576,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>27</v>
@@ -563,7 +590,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>28</v>
@@ -591,7 +618,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>30</v>
@@ -605,7 +632,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>31</v>
@@ -619,7 +646,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>32</v>
@@ -633,7 +660,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>33</v>
@@ -647,7 +674,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
added functionality to show results after uploading them from the file on the frontend
</commit_message>
<xml_diff>
--- a/public/uploads/participants.xlsx
+++ b/public/uploads/participants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6. Mes projets\14.2. Symfony_competition-results\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16241CB-6E11-43AD-BD2B-CC974E4FFDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C692756-F162-4599-AD53-E5BE81BA7C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4188" yWindow="4188" windowWidth="23040" windowHeight="12600" xr2:uid="{A2BB81C9-9CA3-43A5-A119-25B82A2C596C}"/>
+    <workbookView xWindow="4236" yWindow="1644" windowWidth="23040" windowHeight="12600" xr2:uid="{A2BB81C9-9CA3-43A5-A119-25B82A2C596C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Mulhouse</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>Doj</t>
+  </si>
+  <si>
+    <t>Lou</t>
+  </si>
+  <si>
+    <t>Dok</t>
+  </si>
+  <si>
+    <t>lou@gmail.com</t>
+  </si>
+  <si>
+    <t>Brunstatt</t>
   </si>
 </sst>
 </file>
@@ -516,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF053B18-101F-47DE-9D22-6266EEF0E94A}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,6 +695,20 @@
         <v>15</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>